<commit_message>
Plotted new composition data
got sediment composition from Whitney up to samples collected Jan 5 when
I was in Samoa. Still waiting on Meagans new samples
</commit_message>
<xml_diff>
--- a/Data/BulkWeight/Pilot Studies 2012 and 2013-Reef Sediment Traps.xlsx
+++ b/Data/BulkWeight/Pilot Studies 2012 and 2013-Reef Sediment Traps.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\samoa\REEF_SEDIMENT_TRAPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Fagaalu-Sedimentation\Data\BulkWeight\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20055" windowHeight="8160" tabRatio="814" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20055" windowHeight="8160" tabRatio="814" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="february12" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="168">
   <si>
     <t>Number</t>
   </si>
@@ -555,6 +555,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>March 23,2012-March15,2013</t>
   </si>
 </sst>
 </file>
@@ -989,11 +992,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="256398344"/>
-        <c:axId val="256394032"/>
+        <c:axId val="112032376"/>
+        <c:axId val="112035120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="256398344"/>
+        <c:axId val="112032376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1003,7 +1006,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256394032"/>
+        <c:crossAx val="112035120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1011,7 +1014,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256394032"/>
+        <c:axId val="112035120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -1024,7 +1027,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256398344"/>
+        <c:crossAx val="112032376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1204,11 +1207,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="216213856"/>
-        <c:axId val="216208760"/>
+        <c:axId val="515945864"/>
+        <c:axId val="514593952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="216213856"/>
+        <c:axId val="515945864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1251,7 +1254,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216208760"/>
+        <c:crossAx val="514593952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1259,7 +1262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216208760"/>
+        <c:axId val="514593952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1310,7 +1313,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216213856"/>
+        <c:crossAx val="515945864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1523,11 +1526,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="216209152"/>
-        <c:axId val="216206016"/>
+        <c:axId val="514590816"/>
+        <c:axId val="261685376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="216209152"/>
+        <c:axId val="514590816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,7 +1573,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216206016"/>
+        <c:crossAx val="261685376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1578,7 +1581,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216206016"/>
+        <c:axId val="261685376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1629,7 +1632,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216209152"/>
+        <c:crossAx val="514590816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1809,11 +1812,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="256400696"/>
-        <c:axId val="256758952"/>
+        <c:axId val="112031592"/>
+        <c:axId val="112031984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="256400696"/>
+        <c:axId val="112031592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1823,7 +1826,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256758952"/>
+        <c:crossAx val="112031984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1831,7 +1834,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256758952"/>
+        <c:axId val="112031984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -1844,7 +1847,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256400696"/>
+        <c:crossAx val="112031592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2008,11 +2011,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="216216208"/>
-        <c:axId val="216216600"/>
+        <c:axId val="112033552"/>
+        <c:axId val="112034336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="216216208"/>
+        <c:axId val="112033552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2022,7 +2025,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216216600"/>
+        <c:crossAx val="112034336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2030,7 +2033,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216216600"/>
+        <c:axId val="112034336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -2061,7 +2064,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216216208"/>
+        <c:crossAx val="112033552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2219,11 +2222,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="216215032"/>
-        <c:axId val="216217384"/>
+        <c:axId val="515948608"/>
+        <c:axId val="515947040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="216215032"/>
+        <c:axId val="515948608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2233,7 +2236,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216217384"/>
+        <c:crossAx val="515947040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2241,7 +2244,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216217384"/>
+        <c:axId val="515947040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -2254,7 +2257,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216215032"/>
+        <c:crossAx val="515948608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2418,11 +2421,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="216216992"/>
-        <c:axId val="216214248"/>
+        <c:axId val="261683808"/>
+        <c:axId val="261684200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="216216992"/>
+        <c:axId val="261683808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2432,7 +2435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216214248"/>
+        <c:crossAx val="261684200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2440,7 +2443,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216214248"/>
+        <c:axId val="261684200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -2453,7 +2456,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216216992"/>
+        <c:crossAx val="261683808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2614,11 +2617,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="216207584"/>
-        <c:axId val="216212680"/>
+        <c:axId val="261683416"/>
+        <c:axId val="514697400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="216207584"/>
+        <c:axId val="261683416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2628,7 +2631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216212680"/>
+        <c:crossAx val="514697400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2636,7 +2639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216212680"/>
+        <c:axId val="514697400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -2667,7 +2670,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216207584"/>
+        <c:crossAx val="261683416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2865,11 +2868,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="216201704"/>
-        <c:axId val="216204056"/>
+        <c:axId val="514698184"/>
+        <c:axId val="514698968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="216201704"/>
+        <c:axId val="514698184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2879,7 +2882,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216204056"/>
+        <c:crossAx val="514698968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2887,7 +2890,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216204056"/>
+        <c:axId val="514698968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -2900,7 +2903,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216201704"/>
+        <c:crossAx val="514698184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3092,11 +3095,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="216207192"/>
-        <c:axId val="216206800"/>
+        <c:axId val="260987560"/>
+        <c:axId val="260989128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="216207192"/>
+        <c:axId val="260987560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3106,7 +3109,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216206800"/>
+        <c:crossAx val="260989128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3114,7 +3117,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216206800"/>
+        <c:axId val="260989128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -3127,7 +3130,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216207192"/>
+        <c:crossAx val="260987560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3322,11 +3325,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="216211504"/>
-        <c:axId val="216204448"/>
+        <c:axId val="515946256"/>
+        <c:axId val="515947432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="216211504"/>
+        <c:axId val="515946256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3336,7 +3339,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216204448"/>
+        <c:crossAx val="515947432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3344,7 +3347,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216204448"/>
+        <c:axId val="515947432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -3357,7 +3360,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216211504"/>
+        <c:crossAx val="515946256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5627,7 +5630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F16" sqref="F16:K18"/>
     </sheetView>
   </sheetViews>
@@ -6174,7 +6177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
@@ -7868,7 +7871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="Q5" sqref="G1:Q5"/>
     </sheetView>
   </sheetViews>
@@ -13007,7 +13010,7 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13023,7 +13026,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>